<commit_message>
classy c#, level 1, 2, 3
</commit_message>
<xml_diff>
--- a/C# code school cheat sheet.xlsx
+++ b/C# code school cheat sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Try C#</t>
   </si>
@@ -168,13 +168,386 @@
   </si>
   <si>
     <t>CONDITIONALS</t>
+  </si>
+  <si>
+    <t>Getting Classy with C#</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : keyword can be applied to a variable, method or class. It has only one instance per class, the counter is shared. In instances the counter resets.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the advantage of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is, when public, they can be used by other classes without having to create an instance of the class</t>
+    </r>
+  </si>
+  <si>
+    <t>Classes and Objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instance </t>
+  </si>
+  <si>
+    <t>Namespace</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Using directive : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>using System;</t>
+    </r>
+  </si>
+  <si>
+    <t>givesaccess to our System
+Namespace, letting our Compiler know where to
+find Console</t>
+  </si>
+  <si>
+    <t>create an instance of an object</t>
+  </si>
+  <si>
+    <t>ClassName variableName = new ClassName()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access Modifiers / Encapsulation </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> private (default) , protected, internal, public,</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>object initializer</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Groups of Objects</t>
+  </si>
+  <si>
+    <r>
+      <t>Arrays  [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fixed size</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>arrayType[] arrayName = new arrayType</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fixed size</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/dotnet/csharp/programming-guide/arrays/single-dimensional-arrays</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lists</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>variying size</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">arrayType[] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>arrayName = new</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> arrayType[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fixed size</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">need directive </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>using.System.Collections.Generic;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Or use var : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>var variableName = new ClassName()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>List&lt;listType&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> listName = new </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>List&lt;listType&gt;()</t>
+    </r>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>Venue.cs</t>
+  </si>
+  <si>
+    <t>array declaration</t>
+  </si>
+  <si>
+    <t>list declaration</t>
+  </si>
+  <si>
+    <t>adding to list</t>
+  </si>
+  <si>
+    <t>defining array</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,8 +563,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +599,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,18 +618,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -515,6 +931,729 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2301875</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>117413</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12954000"/>
+          <a:ext cx="7175500" cy="3736913"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1764470</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>47214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="17145000"/>
+          <a:ext cx="6638095" cy="3285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1072464</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>66214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7191375" y="17145000"/>
+          <a:ext cx="5485714" cy="3685714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5897657</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1231149</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>177333</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="Group 9"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="17502282" y="17208500"/>
+          <a:ext cx="6033242" cy="3733333"/>
+          <a:chOff x="16200532" y="17208500"/>
+          <a:chExt cx="6033242" cy="3733333"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="8" name="Picture 7"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16224250" y="17208500"/>
+            <a:ext cx="6009524" cy="3733333"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="9" name="Picture 8"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16200532" y="18256251"/>
+            <a:ext cx="5975742" cy="2079626"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1397000</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>742539</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22399625" y="17240251"/>
+          <a:ext cx="6489289" cy="3714749"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1872464</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>110780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7191375" y="21161375"/>
+          <a:ext cx="6285714" cy="2761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>113387</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>104268</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="24622125"/>
+          <a:ext cx="7304762" cy="4057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>349249</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2301562</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7540624" y="24923750"/>
+          <a:ext cx="6365563" cy="2381250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2888339</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>167786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7207250" y="24638000"/>
+          <a:ext cx="7285714" cy="3914286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1151673</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>37619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="34861500"/>
+          <a:ext cx="6819048" cy="3847619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1329417</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>66190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11604625" y="34861500"/>
+          <a:ext cx="7266667" cy="3876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>716869</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>75982</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="25" name="Group 24"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="19954875" y="35480625"/>
+          <a:ext cx="5447619" cy="1742857"/>
+          <a:chOff x="19954875" y="35480625"/>
+          <a:chExt cx="5447619" cy="1742857"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="22" name="Picture 21"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19954875" y="35480625"/>
+            <a:ext cx="5447619" cy="1742857"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="23" name="Picture 22"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="20161249" y="36877624"/>
+            <a:ext cx="1539875" cy="335211"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="24" name="Picture 23"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="20980399" y="36871274"/>
+            <a:ext cx="1539875" cy="335211"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2413000</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>961167</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>82357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14017625" y="22923500"/>
+          <a:ext cx="6866667" cy="1542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1206500</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Arrow Connector 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21129625" y="34766250"/>
+          <a:ext cx="1238250" cy="15875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2381249</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3540124</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>99132</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27066874" y="35242499"/>
+          <a:ext cx="5921375" cy="3909133"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21113750" y="34671000"/>
+          <a:ext cx="6762750" cy="1873250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -807,10 +1946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:L199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="D142" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I200" sqref="I200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,8 +1957,9 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="4" max="4" width="66.28515625" customWidth="1"/>
     <col min="5" max="5" width="89.140625" customWidth="1"/>
+    <col min="11" max="11" width="53.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -888,10 +2028,159 @@
         <v>9</v>
       </c>
     </row>
+    <row r="65" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I90" t="s">
+        <v>19</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D113" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E120" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C155" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C182" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F182" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G182" s="7"/>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B183" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C183" t="s">
+        <v>31</v>
+      </c>
+      <c r="E183" t="s">
+        <v>33</v>
+      </c>
+      <c r="F183" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G183" s="7"/>
+      <c r="H183" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J185" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G186" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L192" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="193" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L193" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="198" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L198" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="199" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L199" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C182" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>